<commit_message>
Support formula, and dynamic column deep link
</commit_message>
<xml_diff>
--- a/public/assets/excel/MostSimpleDatasheet.xlsx
+++ b/public/assets/excel/MostSimpleDatasheet.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Year</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>DeepClone</t>
+  </si>
+  <si>
+    <t>TestNameRange</t>
+  </si>
+  <si>
+    <t>TestForumla</t>
   </si>
 </sst>
 </file>
@@ -398,10 +404,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>25.0</v>
+        <v>32.0</v>
       </c>
       <c r="C4" s="1">
-        <v>32.0</v>
+        <v>21.0</v>
       </c>
       <c r="D4" s="1">
         <v>10.0</v>
@@ -465,6 +471,68 @@
       </c>
       <c r="G6" s="1">
         <v>3250.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <f>zTurnRange</f>
+        <v>-2</v>
+      </c>
+      <c r="C7" s="3">
+        <f>zTurnRange</f>
+        <v>-1</v>
+      </c>
+      <c r="D7" s="3">
+        <f>zTurnRange</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <f>zTurnRange</f>
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <f>zTurnFreeLancer</f>
+        <v>41</v>
+      </c>
+      <c r="G7" s="3">
+        <f>zTurnFreeLancer</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <f>AVERAGE(zTurnFreeLancer)</f>
+        <v>23.5</v>
+      </c>
+      <c r="C8" s="3">
+        <f>MULTIPLY(zTurnRange, zTurnBaseCash)</f>
+        <v>-2000</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ref="D8:F8" si="2">B2:E2</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <f>If(B5 &gt;= G5, B7, G7)</f>
+        <v>5</v>
+      </c>
+      <c r="H8" s="3" t="str">
+        <f>F2:I2</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -531,9 +599,9 @@
         <f>MULTIPLY(zTurnGrowth, zTurnRange)</f>
         <v>0.75</v>
       </c>
-      <c r="G2" s="6" t="str">
-        <f>MULTIPLY(zTurnGrowth, zTurnRange)dfd</f>
-        <v>#ERROR!</v>
+      <c r="G2" s="6">
+        <f>MULTIPLY(zTurnGrowth, zTurnRange)</f>
+        <v>2.2</v>
       </c>
     </row>
     <row r="3">
@@ -541,6 +609,10 @@
         <f>DataSheet!B1</f>
         <v>2007</v>
       </c>
+      <c r="C3" s="3">
+        <f>IF(0&gt;=2, 5, 10)</f>
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update on excel sample sheet
</commit_message>
<xml_diff>
--- a/public/assets/excel/MostSimpleDatasheet.xlsx
+++ b/public/assets/excel/MostSimpleDatasheet.xlsx
@@ -48,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -58,6 +58,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <sz val="11.0"/>
       <color rgb="FF7E3794"/>
@@ -89,7 +90,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -99,12 +100,15 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -383,9 +387,6 @@
       <c r="B3" s="2">
         <v>0.05</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.32</v>
-      </c>
       <c r="D3" s="2">
         <v>0.36</v>
       </c>
@@ -406,8 +407,8 @@
       <c r="B4" s="1">
         <v>32.0</v>
       </c>
-      <c r="C4" s="1">
-        <v>21.0</v>
+      <c r="C4" s="3">
+        <v>0.32</v>
       </c>
       <c r="D4" s="1">
         <v>10.0</v>
@@ -449,23 +450,23 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <f t="shared" ref="B6:F6" si="1">C6</f>
         <v>3250</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <f t="shared" si="1"/>
         <v>3250</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <f t="shared" si="1"/>
         <v>3250</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <f t="shared" si="1"/>
         <v>3250</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <f t="shared" si="1"/>
         <v>3250</v>
       </c>
@@ -477,27 +478,27 @@
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <f>zTurnRange</f>
         <v>-2</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <f>zTurnRange</f>
         <v>-1</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <f>zTurnRange</f>
         <v>1</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <f>zTurnRange</f>
         <v>2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <f>zTurnFreeLancer</f>
         <v>41</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="4">
         <f>zTurnFreeLancer</f>
         <v>5</v>
       </c>
@@ -506,31 +507,31 @@
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <f>AVERAGE(zTurnFreeLancer)</f>
-        <v>23.5</v>
-      </c>
-      <c r="C8" s="3">
+        <v>20.05333333</v>
+      </c>
+      <c r="C8" s="4">
         <f>MULTIPLY(zTurnRange, zTurnBaseCash)</f>
         <v>-2000</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <f t="shared" ref="D8:F8" si="2">B2:E2</f>
         <v>1</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="G8" s="3">
-        <f>If(B5 &gt;= G5, B7, G7)</f>
-        <v>5</v>
-      </c>
-      <c r="H8" s="3" t="str">
+      <c r="G8" s="4">
+        <f>If(B5 &gt;= G5, B7, G7) + D6 * G3</f>
+        <v>1792.5</v>
+      </c>
+      <c r="H8" s="4" t="str">
         <f>F2:I2</f>
         <v/>
       </c>
@@ -551,65 +552,65 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="4">
+      <c r="B1" s="5">
         <f>zTurnRange</f>
         <v>-2</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="5">
         <f>zTurnRange</f>
         <v>-1</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="5">
         <f>zTurnRange</f>
         <v>1</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="5">
         <f>zTurnRange</f>
         <v>2</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="5">
         <f>zTurnRange</f>
         <v>3</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="5">
         <f>zTurnRange</f>
         <v>4</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2">
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <f>IF(zTurnBaseCash &gt; 200, ADD(DataSheet!B3, 5), 0)</f>
         <v>5.05</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <f>IF(zTurnBaseCash &gt; 200, MULTIPLY(zTurnGrowth, 5), 0)</f>
-        <v>1.6</v>
-      </c>
-      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
         <f>MULTIPLY(zTurnGrowth, 5)</f>
         <v>1.8</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="7">
         <f>MULTIPLY(zTurnGrowth, zTurnRange)</f>
         <v>0.3</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <f>MULTIPLY(zTurnGrowth, zTurnRange)</f>
         <v>0.75</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="7">
         <f>MULTIPLY(zTurnGrowth, zTurnRange)</f>
         <v>2.2</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <f>DataSheet!B1</f>
         <v>2007</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <f>IF(0&gt;=2, 5, 10)</f>
         <v>10</v>
       </c>

</xml_diff>